<commit_message>
added volatility calc scripts and GARCH
</commit_message>
<xml_diff>
--- a/ProgressBook.xlsx
+++ b/ProgressBook.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchung\Personal\EquityAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903991D4-F54B-4736-B0F2-2E7CFC1314CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7FF5DB-C46C-4CEF-8165-DBE54237A065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="5100" windowWidth="23620" windowHeight="15700" xr2:uid="{C81E7557-AA14-4D28-85E2-CF30A5309EFF}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="24285" windowHeight="10185" xr2:uid="{C81E7557-AA14-4D28-85E2-CF30A5309EFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="2" r:id="rId1"/>
     <sheet name="Process" sheetId="1" r:id="rId2"/>
     <sheet name="Strategy" sheetId="3" r:id="rId3"/>
+    <sheet name="PromptsToFollowUpOn" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Item</t>
   </si>
@@ -85,7 +86,22 @@
     <t>Found polygon.io for monthly plan</t>
   </si>
   <si>
-    <t>Make a script that measures VaR and cVaR for an equity so I know how it works</t>
+    <t>COMPLETED</t>
+  </si>
+  <si>
+    <t>Make a script that measures VaR and cVaR for an equity so I know how it works. Made another one with stress testing.</t>
+  </si>
+  <si>
+    <t>Make another file that scrolls through all .CSVs to calculate "Portfolio VaR and cVaR" a (e.g. GARCH)nd understand improved mathematical concepts</t>
+  </si>
+  <si>
+    <t>Now pretend you are Warren Buffet. I want to invest in Chinese stocks but want to apply Warren's mindset of long term purchases to a foreign market. Help me understand how Warren would evaluate equities and what considerations he would take into account before buying and his timing of purchases.</t>
+  </si>
+  <si>
+    <t>Provided the answer I expected</t>
+  </si>
+  <si>
+    <t>Created another one that scrolls through all CSVs in folder to calculate portfolio wide and invdidual stats and stress tests. Created a script that forecasts GARCH but doesn't return anything useful. Might have to break it down into pieces.</t>
   </si>
 </sst>
 </file>
@@ -127,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -136,6 +152,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1212,7 +1231,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1347,19 +1366,28 @@
         <v>45567</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>45568</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B15" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>45569</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
@@ -1433,6 +1461,29 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475BACC9-4A7A-4D27-BBB3-E051DBFD0E91}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="100.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{95965d95-ecc0-4720-b759-1f33c42ed7da}" enabled="1" method="Standard" siteId="{a0f29d7e-28cd-4f54-8442-7885aee7c080}" contentBits="0" removed="0"/>

</xml_diff>